<commit_message>
Advanced Excel - For Analysis
</commit_message>
<xml_diff>
--- a/04-диспетчер-сценариев/01-диспетчер-сценариев.xlsx
+++ b/04-диспетчер-сценариев/01-диспетчер-сценариев.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8448" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8448" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="7" r:id="rId1"/>
@@ -17,11 +17,32 @@
     <sheet name="Филиал_инфо" sheetId="5" r:id="rId3"/>
     <sheet name="Модель" sheetId="6" r:id="rId4"/>
     <sheet name="Структура сценария" sheetId="11" r:id="rId5"/>
-    <sheet name="Модель (2)" sheetId="8" r:id="rId6"/>
+    <sheet name="Структура сценария 2" sheetId="12" r:id="rId6"/>
+    <sheet name="Модель (2)" sheetId="8" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="ARPU__руб" localSheetId="6">'Модель (2)'!$B$2</definedName>
+    <definedName name="ARPU__руб">Модель!$B$2</definedName>
+    <definedName name="Абонбаза_на_конец_периода" localSheetId="6">'Модель (2)'!$B$7</definedName>
+    <definedName name="Абонбаза_на_конец_периода">Модель!$B$7</definedName>
+    <definedName name="Абонбаза_на_начало_периода" localSheetId="6">'Модель (2)'!$B$1</definedName>
+    <definedName name="Абонбаза_на_начало_периода">Модель!$B$1</definedName>
+    <definedName name="Отток_абонбазы" localSheetId="6">'Модель (2)'!$B$5</definedName>
+    <definedName name="Отток_абонбазы">Модель!$B$5</definedName>
+    <definedName name="Прирост_абонбазы" localSheetId="6">'Модель (2)'!$B$4</definedName>
+    <definedName name="Прирост_абонбазы">Модель!$B$4</definedName>
+    <definedName name="Расходы_компании" localSheetId="6">'Модель (2)'!$B$3</definedName>
+    <definedName name="Расходы_компании">Модель!$B$3</definedName>
+    <definedName name="Расходы_привлечение_удержание" localSheetId="6">'Модель (2)'!$B$6</definedName>
+    <definedName name="Расходы_привлечение_удержание">Модель!$B$6</definedName>
+    <definedName name="Расчётная_прибыль" localSheetId="6">'Модель (2)'!$B$9</definedName>
+    <definedName name="Расчётная_прибыль">Модель!$B$9</definedName>
+    <definedName name="Условный_доход_за_период" localSheetId="6">'Модель (2)'!$B$8</definedName>
+    <definedName name="Условный_доход_за_период">Модель!$B$8</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="128">
   <si>
     <t>S-1</t>
   </si>
@@ -402,6 +423,21 @@
   <si>
     <t>Автор: user , 04.01.2024
 Автор изменений: user , 04.01.2024</t>
+  </si>
+  <si>
+    <t>ARPU__руб</t>
+  </si>
+  <si>
+    <t>Расходы_компании</t>
+  </si>
+  <si>
+    <t>Расходы_привлечение_удержание</t>
+  </si>
+  <si>
+    <t>Условный_доход_за_период</t>
+  </si>
+  <si>
+    <t>Расчётная_прибыль</t>
   </si>
 </sst>
 </file>
@@ -412,7 +448,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +542,33 @@
     <font>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -610,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -668,6 +731,21 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3242,7 +3320,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Сводная таблица1" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Сводная таблица1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField numFmtId="14" showAll="0"/>
@@ -10251,7 +10329,7 @@
   </sheetPr>
   <dimension ref="B1:F14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10407,6 +10485,169 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="B1:F14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="22.5546875" bestFit="1" customWidth="1" outlineLevel="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="2:6" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="30.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="17">
+        <v>1500</v>
+      </c>
+      <c r="E6" s="27">
+        <v>1200</v>
+      </c>
+      <c r="F6" s="27">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="17">
+        <v>15534789032</v>
+      </c>
+      <c r="E7" s="27">
+        <v>16000832703</v>
+      </c>
+      <c r="F7" s="27">
+        <v>13981310129</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="33"/>
+      <c r="C8" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="17">
+        <v>2746842384</v>
+      </c>
+      <c r="E8" s="27">
+        <v>3433552980</v>
+      </c>
+      <c r="F8" s="27">
+        <v>3433552980</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="17">
+        <v>38072530500</v>
+      </c>
+      <c r="E10" s="17">
+        <v>30458024400</v>
+      </c>
+      <c r="F10" s="17">
+        <v>40610699200</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="35"/>
+      <c r="C11" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="18">
+        <v>19790899084</v>
+      </c>
+      <c r="E11" s="18">
+        <v>11023638717</v>
+      </c>
+      <c r="F11" s="18">
+        <v>23195836091</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>

</xml_diff>